<commit_message>
Added ifoCAST-sampling, changed some settings
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/3_ifo_qoq_series/ifo_qoq_forecasts.xlsx
+++ b/0_0_Data/2_Processed_Data/3_ifo_qoq_series/ifo_qoq_forecasts.xlsx
@@ -380,13 +380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ78"/>
+  <dimension ref="A1:BA82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,8 +543,11 @@
       <c r="AZ1" s="2">
         <v>45800</v>
       </c>
-    </row>
-    <row r="2" spans="1:52">
+      <c r="BA1" s="2">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53">
       <c r="A2" s="2">
         <v>39401</v>
       </c>
@@ -552,7 +555,7 @@
         <v>0.4499999999999886</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:53">
       <c r="A3" s="2">
         <v>39493</v>
       </c>
@@ -560,7 +563,7 @@
         <v>0.2250000000000085</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:53">
       <c r="A4" s="2">
         <v>39583</v>
       </c>
@@ -571,7 +574,7 @@
         <v>-0.3499999999999943</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:53">
       <c r="A5" s="2">
         <v>39675</v>
       </c>
@@ -582,7 +585,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:53">
       <c r="A6" s="2">
         <v>39767</v>
       </c>
@@ -596,7 +599,7 @@
         <v>-0.8999999999999915</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:53">
       <c r="A7" s="2">
         <v>39859</v>
       </c>
@@ -607,7 +610,7 @@
         <v>-0.6500000000000057</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:53">
       <c r="A8" s="2">
         <v>39948</v>
       </c>
@@ -621,7 +624,7 @@
         <v>-0.7000000000000171</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:53">
       <c r="A9" s="2">
         <v>40040</v>
       </c>
@@ -635,7 +638,7 @@
         <v>0.2000000000000028</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:53">
       <c r="A10" s="2">
         <v>40132</v>
       </c>
@@ -652,7 +655,7 @@
         <v>0.4999999999999858</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:53">
       <c r="A11" s="2">
         <v>40224</v>
       </c>
@@ -663,7 +666,7 @@
         <v>0.4200000000000017</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:53">
       <c r="A12" s="2">
         <v>40313</v>
       </c>
@@ -677,7 +680,7 @@
         <v>1.099999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:53">
       <c r="A13" s="2">
         <v>40405</v>
       </c>
@@ -691,7 +694,7 @@
         <v>0.4999999999999858</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:53">
       <c r="A14" s="2">
         <v>40497</v>
       </c>
@@ -708,7 +711,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:53">
       <c r="A15" s="2">
         <v>40589</v>
       </c>
@@ -719,7 +722,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:53">
       <c r="A16" s="2">
         <v>40678</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>0.1206478331785803</v>
       </c>
     </row>
-    <row r="65" spans="1:52">
+    <row r="65" spans="1:53">
       <c r="A65" s="2">
         <v>45153</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="66" spans="1:52">
+    <row r="66" spans="1:53">
       <c r="A66" s="2">
         <v>45245</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>0.044</v>
       </c>
     </row>
-    <row r="67" spans="1:52">
+    <row r="67" spans="1:53">
       <c r="A67" s="2">
         <v>45337</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>-0.08251004046350374</v>
       </c>
     </row>
-    <row r="68" spans="1:52">
+    <row r="68" spans="1:53">
       <c r="A68" s="2">
         <v>45427</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>0.2582525219575302</v>
       </c>
     </row>
-    <row r="69" spans="1:52">
+    <row r="69" spans="1:53">
       <c r="A69" s="2">
         <v>45519</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>-0.04717552522494373</v>
       </c>
     </row>
-    <row r="70" spans="1:52">
+    <row r="70" spans="1:53">
       <c r="A70" s="2">
         <v>45611</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>0.2142297805489477</v>
       </c>
     </row>
-    <row r="71" spans="1:52">
+    <row r="71" spans="1:53">
       <c r="A71" s="2">
         <v>45703</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>0.2394371574146135</v>
       </c>
     </row>
-    <row r="72" spans="1:52">
+    <row r="72" spans="1:53">
       <c r="A72" s="2">
         <v>45792</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>0.04717883418304325</v>
       </c>
     </row>
-    <row r="73" spans="1:52">
+    <row r="73" spans="1:53">
       <c r="A73" s="2">
         <v>45884</v>
       </c>
@@ -1965,8 +1968,11 @@
       <c r="AZ73">
         <v>0.09547648014918764</v>
       </c>
-    </row>
-    <row r="74" spans="1:52">
+      <c r="BA73">
+        <v>0.0959495356205764</v>
+      </c>
+    </row>
+    <row r="74" spans="1:53">
       <c r="A74" s="2">
         <v>45976</v>
       </c>
@@ -1994,8 +2000,11 @@
       <c r="AZ74">
         <v>0.2122469267199563</v>
       </c>
-    </row>
-    <row r="75" spans="1:52">
+      <c r="BA74">
+        <v>0.210242839568366</v>
+      </c>
+    </row>
+    <row r="75" spans="1:53">
       <c r="A75" s="2">
         <v>46068</v>
       </c>
@@ -2011,8 +2020,11 @@
       <c r="AZ75">
         <v>0.3495381990520059</v>
       </c>
-    </row>
-    <row r="76" spans="1:52">
+      <c r="BA75">
+        <v>0.3427795693520892</v>
+      </c>
+    </row>
+    <row r="76" spans="1:53">
       <c r="A76" s="2">
         <v>46157</v>
       </c>
@@ -2028,8 +2040,11 @@
       <c r="AZ76">
         <v>0.4205703094340976</v>
       </c>
-    </row>
-    <row r="77" spans="1:52">
+      <c r="BA76">
+        <v>0.3950901243604932</v>
+      </c>
+    </row>
+    <row r="77" spans="1:53">
       <c r="A77" s="2">
         <v>46249</v>
       </c>
@@ -2045,8 +2060,11 @@
       <c r="AZ77">
         <v>0.4358627554389471</v>
       </c>
-    </row>
-    <row r="78" spans="1:52">
+      <c r="BA77">
+        <v>0.3991974873073616</v>
+      </c>
+    </row>
+    <row r="78" spans="1:53">
       <c r="A78" s="2">
         <v>46341</v>
       </c>
@@ -2061,6 +2079,41 @@
       </c>
       <c r="AZ78">
         <v>0.4473082918826918</v>
+      </c>
+      <c r="BA78">
+        <v>0.411</v>
+      </c>
+    </row>
+    <row r="79" spans="1:53">
+      <c r="A79" s="2">
+        <v>46433</v>
+      </c>
+      <c r="BA79">
+        <v>0.3557500822747528</v>
+      </c>
+    </row>
+    <row r="80" spans="1:53">
+      <c r="A80" s="2">
+        <v>46522</v>
+      </c>
+      <c r="BA80">
+        <v>0.353772834911311</v>
+      </c>
+    </row>
+    <row r="81" spans="1:53">
+      <c r="A81" s="2">
+        <v>46614</v>
+      </c>
+      <c r="BA81">
+        <v>0.3196762671417588</v>
+      </c>
+    </row>
+    <row r="82" spans="1:53">
+      <c r="A82" s="2">
+        <v>46706</v>
+      </c>
+      <c r="BA82">
+        <v>0.2871413350329135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>